<commit_message>
SQL Server Compatibility and Password Policies
- Created two SQL scripts - one for MySQL and one for SQL Server
- Updated app.py (with some commented lines that can be uncommented) to be compatible with SQL Server
- Updated requirements.txt for SQL Server compatibility
- Added password policies requiring a minimum of 8 characters, a number, a special character, and an uppercase letter.
- Updated error handling for invalid passwords
- Added audit logging when failing to create/update user with invalid password
- Added JS and HTML button to toggle password visibility on user dashboard (hidden by default)
</commit_message>
<xml_diff>
--- a/Documentation/Event_Logging.xlsx
+++ b/Documentation/Event_Logging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/slk125_pitt_edu/Documents/24-25 Spring/CIST 1451/Github/CAPSTONE-Password-Manager/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{9A701678-90BC-4C5B-8261-7BD62605C600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{605B0A12-CAD2-4420-AECC-C6639B790511}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{9A701678-90BC-4C5B-8261-7BD62605C600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6325C568-186B-42CD-9576-79F606343C4F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B89527-BBF8-46ED-8D81-27FC1D6BCF40}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Event</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Failed to View Audit Logs (Unauthorized)</t>
+  </si>
+  <si>
+    <t>Failed to Create User (Invalid Password)</t>
+  </si>
+  <si>
+    <t>Failed to Update User (Invalid Password)</t>
   </si>
 </sst>
 </file>
@@ -116,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +143,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -163,11 +175,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -184,6 +197,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -503,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB59255-DE4D-425A-9550-27ED5E74C070}">
-  <dimension ref="B2:C18"/>
+  <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,58 +614,74 @@
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="C19" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>